<commit_message>
$w should create assigner property, not source.
</commit_message>
<xml_diff>
--- a/spec/ConvSpec-760-788-Links-v1.6.xlsx
+++ b/spec/ConvSpec-760-788-Links-v1.6.xlsx
@@ -468,9 +468,6 @@
     <t>Bk-499; Se-30K</t>
   </si>
   <si>
-    <t>If $w begins with (DLC), I - identified by - Lccn - rdf:value "number without (DLC)" and ## - source - Source - http://id.loc.gov/vocabulary/organizations/dlc ; else I - identifiedBy - Identifier - rdf:value "number without data in parens" and ## - source - Source - bf:code (data in parentheses)</t>
-  </si>
-  <si>
     <t>W - bflc:relationship - bflc:Relationship - bflc:relation - bflc:Relation - rdfs:label "content of $i".  See also Process 0.3.3</t>
   </si>
   <si>
@@ -522,11 +519,14 @@
     <t>Create a new Instance and link it to the current resource</t>
   </si>
   <si>
-    <t xml:space="preserve">Fields 76X-78X - Linking Entries - v1.6, 11/24/2020
+    <t>I - title - Title - mainTitle - literal ; use Instance title from MARC 245 if no $t exists</t>
+  </si>
+  <si>
+    <t>If $w begins with (DLC), I - identified by - Lccn - rdf:value "number without (DLC)" and ## - assigner - Agent - http://id.loc.gov/vocabulary/organizations/dlc ; else I - identifiedBy - Identifier - rdf:value "number without data in parens" and ## - assigner - Agent - bf:code (data in parentheses)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fields 76X-78X - Linking Entries - v1.6, 12/01/2020
 </t>
-  </si>
-  <si>
-    <t>I - title - Title - mainTitle - literal ; use Instance title from MARC 245 if no $t exists</t>
   </si>
 </sst>
 </file>
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -980,7 +980,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -989,7 +989,7 @@
         <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>111</v>
@@ -1001,13 +1001,13 @@
     <row r="3" spans="1:8" s="1" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H3" s="9"/>
     </row>
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1034,7 +1034,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1129,14 +1129,14 @@
       </c>
       <c r="B14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>121</v>
       </c>
       <c r="F14" s="3"/>
       <c r="H14" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1152,7 +1152,7 @@
         <v>122</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1492,10 +1492,10 @@
         <v>70</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="31" x14ac:dyDescent="0.35">
@@ -1559,13 +1559,13 @@
         <v>8</v>
       </c>
       <c r="B55" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
@@ -1634,10 +1634,10 @@
         <v>70</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="31" x14ac:dyDescent="0.35">
@@ -1645,7 +1645,7 @@
         <v>34</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>70</v>
@@ -1676,10 +1676,10 @@
         <v>70</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1701,13 +1701,13 @@
         <v>13</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="31" x14ac:dyDescent="0.35">
@@ -1745,11 +1745,11 @@
       <c r="B68" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>144</v>
+      <c r="C68" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="31" x14ac:dyDescent="0.35">
@@ -1757,7 +1757,7 @@
         <v>15</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>70</v>
@@ -1813,13 +1813,13 @@
         <v>17</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>